<commit_message>
Add start of BOM, kp layout, etc
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -5,20 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frank\Documents\repos\binulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francis\Documents\repos\binulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAFC2C8-CD0F-4A60-94D1-44BF76719A9A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49017A58-85E5-4029-91A2-9FDC1A1BFADD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{AB5CF698-8B4B-4CB6-BC5E-910315228B51}"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{DD5D3D6A-3E87-44D1-913F-F29D543648C7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="5" xr2:uid="{AB5CF698-8B4B-4CB6-BC5E-910315228B51}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{DD5D3D6A-3E87-44D1-913F-F29D543648C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Keymap" sheetId="1" r:id="rId1"/>
     <sheet name="Key_Layout" sheetId="5" r:id="rId2"/>
     <sheet name="Pin Count" sheetId="4" r:id="rId3"/>
     <sheet name="BOM" sheetId="2" r:id="rId4"/>
-    <sheet name="Pin Mux" sheetId="3" r:id="rId5"/>
+    <sheet name="power estimate" sheetId="7" r:id="rId5"/>
+    <sheet name="display layout" sheetId="6" r:id="rId6"/>
+    <sheet name="Pin Mux" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -70,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="244">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -466,6 +468,342 @@
   </si>
   <si>
     <t>Clear Selected</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Part Name</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Cost per unit</t>
+  </si>
+  <si>
+    <t>QTY per device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost </t>
+  </si>
+  <si>
+    <t>Postage cost</t>
+  </si>
+  <si>
+    <t>PIXEL dims</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>px</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>Operating voltage</t>
+  </si>
+  <si>
+    <t>3.3V</t>
+  </si>
+  <si>
+    <t>proposed</t>
+  </si>
+  <si>
+    <t>SPI interface</t>
+  </si>
+  <si>
+    <t>https://core-electronics.com.au/50-pin-0-5mm-pitch-top-contact-fpc-smt-connector.html</t>
+  </si>
+  <si>
+    <t>Display connector</t>
+  </si>
+  <si>
+    <t>https://core-electronics.com.au/2-8-tft-display-with-resistive-touchscreen.html?utm_source=google_shopping&amp;gclid=CjwKCAjwzqPcBRAnEiwAzKRgS9iknk_lDDactmHV8T55h4Bo84qGHhKtobF5cuqon29wsBr49jb8XBoCZbAQAvD_BwE</t>
+  </si>
+  <si>
+    <t>2.8 TFT Display with Resistive Touchscreen</t>
+  </si>
+  <si>
+    <t>Display PINS</t>
+  </si>
+  <si>
+    <t>Interface to ILI9341 driver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIN NAME </t>
+  </si>
+  <si>
+    <t>VDDI</t>
+  </si>
+  <si>
+    <t>VDDI_LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Will we use this? </t>
+  </si>
+  <si>
+    <t>VCI</t>
+  </si>
+  <si>
+    <t>Analog power</t>
+  </si>
+  <si>
+    <t>Vcore</t>
+  </si>
+  <si>
+    <t>Regulated output</t>
+  </si>
+  <si>
+    <t>IM3:0</t>
+  </si>
+  <si>
+    <t>MCU ifce mode</t>
+  </si>
+  <si>
+    <t>0x0000</t>
+  </si>
+  <si>
+    <t>MEANING pins D[7:0]</t>
+  </si>
+  <si>
+    <t>D7:0</t>
+  </si>
+  <si>
+    <t>parallel input bus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESX </t>
+  </si>
+  <si>
+    <t>Active low</t>
+  </si>
+  <si>
+    <t>Connect to GND for operation</t>
+  </si>
+  <si>
+    <t>EXTC</t>
+  </si>
+  <si>
+    <t>extended command set</t>
+  </si>
+  <si>
+    <t>LOGIC PINS</t>
+  </si>
+  <si>
+    <t>DESC</t>
+  </si>
+  <si>
+    <t>SOURCES</t>
+  </si>
+  <si>
+    <t>DIR (IN/OUT)</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>NOTE</t>
+  </si>
+  <si>
+    <t>VDDI/VSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN ESSENTIAL? </t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>MCU</t>
+  </si>
+  <si>
+    <t>MCU?</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>TBC?</t>
+  </si>
+  <si>
+    <t>TBC</t>
+  </si>
+  <si>
+    <t>CSX</t>
+  </si>
+  <si>
+    <t>chip select input pin</t>
+  </si>
+  <si>
+    <t>No effect on disp mod in parallel mod</t>
+  </si>
+  <si>
+    <t>D/CX (DCX)</t>
+  </si>
+  <si>
+    <t>data/command switch</t>
+  </si>
+  <si>
+    <t>Needed for || mode</t>
+  </si>
+  <si>
+    <t>RDX</t>
+  </si>
+  <si>
+    <t>WRX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TBC? </t>
+  </si>
+  <si>
+    <t>8080-I/II system write signal</t>
+  </si>
+  <si>
+    <t>D17:8</t>
+  </si>
+  <si>
+    <t>Conn to VSS</t>
+  </si>
+  <si>
+    <t>SDI/SDA</t>
+  </si>
+  <si>
+    <t>8080 read signal</t>
+  </si>
+  <si>
+    <t>8080 write signal</t>
+  </si>
+  <si>
+    <t>IN/OUT</t>
+  </si>
+  <si>
+    <t>Serial IO signal</t>
+  </si>
+  <si>
+    <t>SDO</t>
+  </si>
+  <si>
+    <t>Serial output signal</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>if unused open the pin</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>TE</t>
+  </si>
+  <si>
+    <t>tearing effect output pin</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>what is this</t>
+  </si>
+  <si>
+    <t>DOTCLK</t>
+  </si>
+  <si>
+    <t>dot clock signal for RGB interface operation</t>
+  </si>
+  <si>
+    <t>Not sure</t>
+  </si>
+  <si>
+    <t>VSYNC</t>
+  </si>
+  <si>
+    <t>HSYNC</t>
+  </si>
+  <si>
+    <t>frame sync for RGB</t>
+  </si>
+  <si>
+    <t>line sync for RGB</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>data enable for RGB mode=</t>
+  </si>
+  <si>
+    <t>8080-I/II system read signal</t>
+  </si>
+  <si>
+    <t>GROUP</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Unused</t>
+  </si>
+  <si>
+    <t>RGB ifce</t>
+  </si>
+  <si>
+    <t>https://au.mouser.com/ProductDetail/TE-Connectivity-Alcoswitch/FSM2JRT?qs=sGAEpiMZZMtFyPk3yBMYYCyhGENGH2NPU1ol7T%2fXypo%3d</t>
+  </si>
+  <si>
+    <t>switches</t>
+  </si>
+  <si>
+    <t>https://au.mouser.com/ProductDetail/STMicroelectronics/STM32F101VCT6?qs=sGAEpiMZZMuoKKEcg8mMKEEgaNexwACoO9ADMQn40mU%3d</t>
+  </si>
+  <si>
+    <t>MCU - STMicroelectronics STM32F101VCT6</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage </t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>LCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUTTONS </t>
+  </si>
+  <si>
+    <t>Calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEDS </t>
+  </si>
+  <si>
+    <t>LCD driver</t>
+  </si>
+  <si>
+    <t>https://au.mouser.com/ProductDetail/ROHM-Semiconductor/BU33SD5WG-TR?qs=sGAEpiMZZMsMIqGZiACxIdSGhSU%252b3GFE32FMIpI1rfZTloTAi0PROQ%3d%3d</t>
+  </si>
+  <si>
+    <t>3.3V voltage regulator</t>
+  </si>
+  <si>
+    <t>USB connector</t>
+  </si>
+  <si>
+    <t>https://au.mouser.com/ProductDetail/Amphenol-FCI/10118193-0001LF?qs=sGAEpiMZZMuhucAexPYLesFMAgXhqips</t>
   </si>
 </sst>
 </file>
@@ -494,12 +832,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -662,7 +1012,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -678,6 +1028,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -994,10 +1348,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D03D7666-294F-443D-BB17-A232AE17218E}">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView topLeftCell="A29" workbookViewId="1">
+      <selection activeCell="A47" sqref="A47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2638,10 +2994,10 @@
   <dimension ref="A4:X86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="Z15" sqref="Z15"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6692,7 +7048,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -6754,20 +7110,823 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EF524C-A33F-43D3-860D-46F0F9167D43}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:B40"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="67.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2">
+        <v>30.5</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>D2*E2+F2</f>
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3">
+        <v>3.5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G7" si="0">D3*E3+F3</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D4">
+        <v>0.151</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>0.01</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>7.56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D5">
+        <v>9.06</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0.01</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>9.07</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>241</v>
+      </c>
+      <c r="C6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D6">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0.01</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0.57699999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>242</v>
+      </c>
+      <c r="C7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D7">
+        <v>0.61</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0.01</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>231</v>
+      </c>
+      <c r="G13">
+        <f>SUM(G2:G12)</f>
+        <v>51.826999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113F1A7A-9196-48A1-BEB8-1076D278492A}">
+  <dimension ref="A2:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3">
+        <v>3.3</v>
+      </c>
+      <c r="D3" s="15">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D4" s="15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D5" s="15"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>238</v>
+      </c>
+      <c r="B7">
+        <f>4*20</f>
+        <v>80</v>
+      </c>
+      <c r="D7">
+        <f>B7*0.001</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>231</v>
+      </c>
+      <c r="D8" s="16">
+        <f>SUM(D3:D7)</f>
+        <v>0.33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86508168-602A-4B3E-8914-51A2FB7F6D83}">
+  <dimension ref="A1:H40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2">
+        <v>264</v>
+      </c>
+      <c r="D2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3">
+        <v>176</v>
+      </c>
+      <c r="D3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>154</v>
+      </c>
+      <c r="C19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20">
+        <v>3.3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>157</v>
+      </c>
+      <c r="C21">
+        <v>3.3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>159</v>
+      </c>
+      <c r="D22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>172</v>
+      </c>
+      <c r="B24" t="s">
+        <v>223</v>
+      </c>
+      <c r="C24" t="s">
+        <v>173</v>
+      </c>
+      <c r="D24" t="s">
+        <v>174</v>
+      </c>
+      <c r="E24" t="s">
+        <v>179</v>
+      </c>
+      <c r="F24" t="s">
+        <v>175</v>
+      </c>
+      <c r="G24" t="s">
+        <v>176</v>
+      </c>
+      <c r="H24" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="C25" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" t="s">
+        <v>178</v>
+      </c>
+      <c r="E25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F25" t="s">
+        <v>183</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="H25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="C26" t="s">
+        <v>166</v>
+      </c>
+      <c r="D26" t="s">
+        <v>178</v>
+      </c>
+      <c r="E26" t="s">
+        <v>180</v>
+      </c>
+      <c r="F26" t="s">
+        <v>201</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B27" t="s">
+        <v>225</v>
+      </c>
+      <c r="C27" t="s">
+        <v>166</v>
+      </c>
+      <c r="D27" t="s">
+        <v>178</v>
+      </c>
+      <c r="E27" t="s">
+        <v>180</v>
+      </c>
+      <c r="F27" t="s">
+        <v>201</v>
+      </c>
+      <c r="G27" s="13">
+        <v>0</v>
+      </c>
+      <c r="H27" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" t="s">
+        <v>168</v>
+      </c>
+      <c r="D28" t="s">
+        <v>178</v>
+      </c>
+      <c r="E28" t="s">
+        <v>180</v>
+      </c>
+      <c r="F28" t="s">
+        <v>183</v>
+      </c>
+      <c r="G28" t="s">
+        <v>182</v>
+      </c>
+      <c r="H28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>170</v>
+      </c>
+      <c r="C29" t="s">
+        <v>171</v>
+      </c>
+      <c r="D29" t="s">
+        <v>178</v>
+      </c>
+      <c r="E29" t="s">
+        <v>180</v>
+      </c>
+      <c r="F29" t="s">
+        <v>183</v>
+      </c>
+      <c r="G29" t="s">
+        <v>184</v>
+      </c>
+      <c r="H29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B30" s="13">
+        <v>8080</v>
+      </c>
+      <c r="C30" t="s">
+        <v>187</v>
+      </c>
+      <c r="D30" t="s">
+        <v>178</v>
+      </c>
+      <c r="E30" t="s">
+        <v>180</v>
+      </c>
+      <c r="F30" t="s">
+        <v>183</v>
+      </c>
+      <c r="G30" s="13">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="B31" s="13">
+        <v>8080</v>
+      </c>
+      <c r="C31" t="s">
+        <v>190</v>
+      </c>
+      <c r="D31" t="s">
+        <v>178</v>
+      </c>
+      <c r="E31" t="s">
+        <v>180</v>
+      </c>
+      <c r="F31" t="s">
+        <v>183</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="H31" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="B32" s="13">
+        <v>8080</v>
+      </c>
+      <c r="C32" t="s">
+        <v>199</v>
+      </c>
+      <c r="D32" t="s">
+        <v>178</v>
+      </c>
+      <c r="E32" t="s">
+        <v>180</v>
+      </c>
+      <c r="F32" t="s">
+        <v>183</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="H32" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="B33" s="13">
+        <v>8080</v>
+      </c>
+      <c r="C33" t="s">
+        <v>200</v>
+      </c>
+      <c r="D33" t="s">
+        <v>178</v>
+      </c>
+      <c r="E33" t="s">
+        <v>180</v>
+      </c>
+      <c r="F33" t="s">
+        <v>183</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="H33" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>198</v>
+      </c>
+      <c r="C34" t="s">
+        <v>202</v>
+      </c>
+      <c r="D34" t="s">
+        <v>178</v>
+      </c>
+      <c r="E34" t="s">
+        <v>180</v>
+      </c>
+      <c r="F34" t="s">
+        <v>201</v>
+      </c>
+      <c r="G34" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>203</v>
+      </c>
+      <c r="C35" t="s">
+        <v>204</v>
+      </c>
+      <c r="D35" t="s">
+        <v>178</v>
+      </c>
+      <c r="E35" t="s">
+        <v>207</v>
+      </c>
+      <c r="F35" t="s">
+        <v>205</v>
+      </c>
+      <c r="G35" t="s">
+        <v>182</v>
+      </c>
+      <c r="H35" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>208</v>
+      </c>
+      <c r="C36" t="s">
+        <v>209</v>
+      </c>
+      <c r="D36" t="s">
+        <v>178</v>
+      </c>
+      <c r="E36" t="s">
+        <v>210</v>
+      </c>
+      <c r="F36" t="s">
+        <v>205</v>
+      </c>
+      <c r="G36" t="s">
+        <v>182</v>
+      </c>
+      <c r="H36" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B37" t="s">
+        <v>226</v>
+      </c>
+      <c r="C37" t="s">
+        <v>213</v>
+      </c>
+      <c r="D37" t="s">
+        <v>178</v>
+      </c>
+      <c r="E37" t="s">
+        <v>180</v>
+      </c>
+      <c r="F37" t="s">
+        <v>183</v>
+      </c>
+      <c r="H37" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B38" t="s">
+        <v>226</v>
+      </c>
+      <c r="C38" t="s">
+        <v>217</v>
+      </c>
+      <c r="D38" t="s">
+        <v>178</v>
+      </c>
+      <c r="E38" t="s">
+        <v>180</v>
+      </c>
+      <c r="F38" t="s">
+        <v>183</v>
+      </c>
+      <c r="H38" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="B39" t="s">
+        <v>226</v>
+      </c>
+      <c r="C39" t="s">
+        <v>218</v>
+      </c>
+      <c r="D39" t="s">
+        <v>178</v>
+      </c>
+      <c r="E39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F39" t="s">
+        <v>183</v>
+      </c>
+      <c r="H39" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>220</v>
+      </c>
+      <c r="C40" t="s">
+        <v>221</v>
+      </c>
+      <c r="D40" t="s">
+        <v>178</v>
+      </c>
+      <c r="E40" t="s">
+        <v>180</v>
+      </c>
+      <c r="F40" t="s">
+        <v>183</v>
+      </c>
+      <c r="H40" t="s">
+        <v>219</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895AF181-FBD3-4423-B9E0-C4D4707FE481}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
latest version of the docs
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,9 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francis\Documents\repos\binulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49017A58-85E5-4029-91A2-9FDC1A1BFADD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C0D98E-56CE-4AB2-A6E7-11459ABD9534}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="5" xr2:uid="{AB5CF698-8B4B-4CB6-BC5E-910315228B51}"/>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{DD5D3D6A-3E87-44D1-913F-F29D543648C7}"/>
   </bookViews>
   <sheets>
@@ -810,7 +809,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -830,6 +829,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1009,10 +1016,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1032,8 +1040,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1348,10 +1358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D03D7666-294F-443D-BB17-A232AE17218E}">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
-    </sheetView>
-    <sheetView topLeftCell="A29" workbookViewId="1">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
@@ -2994,9 +3001,6 @@
   <dimension ref="A4:X86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Z15" sqref="Z15"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -7047,10 +7051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11910E8F-F881-4FEF-8DE8-B91E27082970}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7112,11 +7113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EF524C-A33F-43D3-860D-46F0F9167D43}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:B40"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7207,7 +7205,7 @@
       <c r="B4" t="s">
         <v>228</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="17" t="s">
         <v>227</v>
       </c>
       <c r="D4">
@@ -7306,8 +7304,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{62094591-22EE-4986-A182-297BA690668C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7315,8 +7316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113F1A7A-9196-48A1-BEB8-1076D278492A}">
   <dimension ref="A2:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -7405,10 +7405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86508168-602A-4B3E-8914-51A2FB7F6D83}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7931,7 +7928,6 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Add links to datasheets
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francis\Documents\repos\binulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dktrfrd0/Documents/repos/binulator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C0D98E-56CE-4AB2-A6E7-11459ABD9534}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCC4787-C848-8748-93DB-881C9D283555}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{DD5D3D6A-3E87-44D1-913F-F29D543648C7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12220" activeTab="3" xr2:uid="{DD5D3D6A-3E87-44D1-913F-F29D543648C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Keymap" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="display layout" sheetId="6" r:id="rId6"/>
     <sheet name="Pin Mux" sheetId="3" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="247">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -803,6 +803,15 @@
   </si>
   <si>
     <t>https://au.mouser.com/ProductDetail/Amphenol-FCI/10118193-0001LF?qs=sGAEpiMZZMuhucAexPYLesFMAgXhqips</t>
+  </si>
+  <si>
+    <t>dsheet</t>
+  </si>
+  <si>
+    <t>https://au.mouser.com/datasheet/2/389/stm32f101rc-956301.pdf</t>
+  </si>
+  <si>
+    <t>https://cdn-shop.adafruit.com/datasheets/62684.pdf</t>
   </si>
 </sst>
 </file>
@@ -1362,23 +1371,23 @@
       <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.5" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -1395,7 +1404,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>45</v>
       </c>
@@ -1433,7 +1442,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -1464,7 +1473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1495,7 +1504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1526,7 +1535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1557,7 +1566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1588,7 +1597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1619,7 +1628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1650,7 +1659,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1681,7 +1690,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1712,7 +1721,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1743,7 +1752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1774,7 +1783,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1805,7 +1814,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1836,7 +1845,7 @@
         <v>C</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -1867,7 +1876,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1898,7 +1907,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1925,7 +1934,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1954,7 +1963,7 @@
         <v>=</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1991,7 +2000,7 @@
         <v>+ (RL)</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -2028,7 +2037,7 @@
         <v>- (RR)</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -2065,7 +2074,7 @@
         <v>/ (&gt;&gt;)</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -2102,7 +2111,7 @@
         <v>* (&lt;&lt;)</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -2129,7 +2138,7 @@
         <v>%</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -2166,7 +2175,7 @@
         <v>| (~)</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -2203,7 +2212,7 @@
         <v>&amp; (^)</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -2230,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -2257,7 +2266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -2288,7 +2297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -2319,7 +2328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -2350,7 +2359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -2381,7 +2390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>30</v>
       </c>
@@ -2412,7 +2421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>31</v>
       </c>
@@ -2443,7 +2452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>32</v>
       </c>
@@ -2474,7 +2483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>33</v>
       </c>
@@ -2515,7 +2524,7 @@
         <v>DEC (W8)</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>34</v>
       </c>
@@ -2556,7 +2565,7 @@
         <v>OCT (W16)</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>35</v>
       </c>
@@ -2597,7 +2606,7 @@
         <v>HEX (W32)</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>36</v>
       </c>
@@ -2638,7 +2647,7 @@
         <v>BIN (W64)</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>37</v>
       </c>
@@ -2671,7 +2680,7 @@
         <v>CS</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>38</v>
       </c>
@@ -2704,7 +2713,7 @@
         <v>CA</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>39</v>
       </c>
@@ -2745,7 +2754,7 @@
         <v>/\ (Menu)</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>40</v>
       </c>
@@ -2778,7 +2787,7 @@
         <v>\/</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>41</v>
       </c>
@@ -2811,7 +2820,7 @@
         <v>&lt;</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>42</v>
       </c>
@@ -2844,7 +2853,7 @@
         <v>&gt;</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>43</v>
       </c>
@@ -2877,7 +2886,7 @@
         <v>R-&gt;A</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>44</v>
       </c>
@@ -2910,7 +2919,7 @@
         <v>R-&gt;B</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>45</v>
       </c>
@@ -2943,7 +2952,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>46</v>
       </c>
@@ -2976,7 +2985,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>115</v>
       </c>
@@ -2985,7 +2994,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>116</v>
       </c>
@@ -3004,12 +3013,12 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="13" max="24" width="9.5703125" customWidth="1"/>
+    <col min="13" max="24" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -3017,7 +3026,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="E5" s="6" t="s">
         <v>43</v>
       </c>
@@ -3091,7 +3100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="G6" t="s">
         <v>76</v>
       </c>
@@ -3156,7 +3165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="G7" t="s">
         <v>46</v>
       </c>
@@ -3218,7 +3227,7 @@
         <v>&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="G8" t="s">
         <v>6</v>
       </c>
@@ -3280,7 +3289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="G9" t="s">
         <v>3</v>
       </c>
@@ -3339,7 +3348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="G10">
         <v>7</v>
       </c>
@@ -3404,7 +3413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="G11">
         <v>4</v>
       </c>
@@ -3469,7 +3478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="G12">
         <v>1</v>
       </c>
@@ -3534,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="G13">
         <v>0</v>
       </c>
@@ -3596,7 +3605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="M14" s="12">
         <f>VLOOKUP(A14,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -3646,7 +3655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="M15" s="12">
         <f>VLOOKUP(A15,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -3696,7 +3705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="M16" s="12">
         <f>VLOOKUP(A16,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -3746,7 +3755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M17" s="12">
         <f>VLOOKUP(A17,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -3796,7 +3805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M18" s="12">
         <f>VLOOKUP(A18,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -3846,7 +3855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M19" s="12">
         <f>VLOOKUP(A19,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -3896,7 +3905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M20" s="12">
         <f>VLOOKUP(A20,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -3946,7 +3955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M21" s="12">
         <f>VLOOKUP(A21,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -3996,7 +4005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M22" s="12">
         <f>VLOOKUP(A22,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4046,7 +4055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M23" s="12">
         <f>VLOOKUP(A23,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4096,7 +4105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M24" s="12">
         <f>VLOOKUP(A24,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4146,7 +4155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M25" s="12">
         <f>VLOOKUP(A25,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4196,7 +4205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M26" s="12">
         <f>VLOOKUP(A26,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4246,7 +4255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M27" s="12">
         <f>VLOOKUP(A27,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4296,7 +4305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M28" s="12">
         <f>VLOOKUP(A28,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4346,7 +4355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M29" s="12">
         <f>VLOOKUP(A29,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4396,7 +4405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M30" s="12">
         <f>VLOOKUP(A30,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4446,7 +4455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M31" s="12">
         <f>VLOOKUP(A31,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4496,7 +4505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M32" s="12">
         <f>VLOOKUP(A32,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4546,7 +4555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M33" s="12">
         <f>VLOOKUP(A33,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4596,7 +4605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M34" s="12">
         <f>VLOOKUP(A34,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4646,7 +4655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M35">
         <f>VLOOKUP(A35,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4696,7 +4705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M36">
         <f>VLOOKUP(A36,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -4742,7 +4751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M37">
         <f>VLOOKUP(A37,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -4788,7 +4797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M38">
         <f>VLOOKUP(A38,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -4834,7 +4843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M39">
         <f>VLOOKUP(A39,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -4880,7 +4889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M40">
         <f>VLOOKUP(A40,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -4926,7 +4935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M41">
         <f>VLOOKUP(A41,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -4972,7 +4981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M42">
         <f>VLOOKUP(A42,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5018,7 +5027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M43">
         <f>VLOOKUP(A43,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5064,7 +5073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M44">
         <f>VLOOKUP(A44,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5110,7 +5119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M45">
         <f>VLOOKUP(A45,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5156,7 +5165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M46">
         <f>VLOOKUP(A46,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5202,7 +5211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M47">
         <f>VLOOKUP(A47,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5248,7 +5257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="13:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="13:24" x14ac:dyDescent="0.2">
       <c r="M48">
         <f>VLOOKUP(A48,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5294,7 +5303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M49">
         <f>VLOOKUP(A49,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5340,7 +5349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M50">
         <f>VLOOKUP(A50,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5386,7 +5395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M51">
         <f>VLOOKUP(A51,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5432,7 +5441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M52">
         <f>VLOOKUP(A52,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5478,7 +5487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M53">
         <f>VLOOKUP(A53,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5524,7 +5533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M54">
         <f>VLOOKUP(A54,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5570,7 +5579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M55">
         <f>VLOOKUP(A55,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5616,7 +5625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M56">
         <f>VLOOKUP(A56,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5662,7 +5671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M57">
         <f>VLOOKUP(A57,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5708,7 +5717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M58">
         <f>VLOOKUP(A58,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5754,7 +5763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M59">
         <f>VLOOKUP(A59,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5800,7 +5809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M60">
         <f>VLOOKUP(A60,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5846,7 +5855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M61">
         <f>VLOOKUP(A61,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5892,7 +5901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M62">
         <f>VLOOKUP(A62,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5938,7 +5947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M63">
         <f>VLOOKUP(A63,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5984,7 +5993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M64">
         <f>VLOOKUP(A64,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6030,7 +6039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M65">
         <f>VLOOKUP(A65,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6076,7 +6085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M66">
         <f>VLOOKUP(A66,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6122,7 +6131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M67">
         <f>VLOOKUP(A67,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6168,7 +6177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M68">
         <f>VLOOKUP(A68,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6214,7 +6223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M69">
         <f>VLOOKUP(A69,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6260,7 +6269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M70">
         <f>VLOOKUP(A70,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6306,7 +6315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M71">
         <f>VLOOKUP(A71,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6352,7 +6361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M72">
         <f>VLOOKUP(A72,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6398,7 +6407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M73">
         <f>VLOOKUP(A73,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6444,7 +6453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M74">
         <f>VLOOKUP(A74,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6490,7 +6499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M75">
         <f>VLOOKUP(A75,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6536,7 +6545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M76">
         <f>VLOOKUP(A76,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6582,7 +6591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="77" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M77">
         <f>VLOOKUP(A77,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6628,7 +6637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="78" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M78">
         <f>VLOOKUP(A78,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6674,7 +6683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="79" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M79">
         <f>VLOOKUP(A79,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6720,7 +6729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="80" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M80">
         <f>VLOOKUP(A80,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6766,7 +6775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M81">
         <f>VLOOKUP(A81,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6812,7 +6821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="82" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M82">
         <f>VLOOKUP(A82,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6858,7 +6867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M83">
         <f>VLOOKUP(A83,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6904,7 +6913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="84" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M84">
         <f>VLOOKUP(A84,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6950,7 +6959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="85" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M85">
         <f>VLOOKUP(A85,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6996,7 +7005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="86" spans="13:23" x14ac:dyDescent="0.2">
       <c r="M86">
         <f>VLOOKUP(A86,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -7053,12 +7062,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -7072,7 +7081,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>117</v>
       </c>
@@ -7084,7 +7093,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>122</v>
       </c>
@@ -7095,7 +7104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>123</v>
       </c>
@@ -7111,23 +7120,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EF524C-A33F-43D3-860D-46F0F9167D43}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="67.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="182.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="182.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>132</v>
       </c>
@@ -7138,19 +7149,22 @@
         <v>134</v>
       </c>
       <c r="D1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E1" t="s">
         <v>135</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>136</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>138</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -7160,21 +7174,21 @@
       <c r="C2" t="s">
         <v>149</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>30.5</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
       <c r="G2">
-        <f>D2*E2+F2</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>E2*F2+G2</f>
         <v>30.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -7184,21 +7198,24 @@
       <c r="C3" t="s">
         <v>147</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E3">
         <v>3.5</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
       <c r="G3">
-        <f t="shared" ref="G3:G7" si="0">D3*E3+F3</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H7" si="0">E3*F3+G3</f>
         <v>3.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -7208,21 +7225,22 @@
       <c r="C4" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="17"/>
+      <c r="E4">
         <v>0.151</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>50</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.01</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <f t="shared" si="0"/>
         <v>7.56</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -7232,21 +7250,24 @@
       <c r="C5" t="s">
         <v>229</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E5">
         <v>9.06</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.01</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <f t="shared" si="0"/>
         <v>9.07</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -7256,21 +7277,21 @@
       <c r="C6" t="s">
         <v>240</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0.56699999999999995</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.01</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <f t="shared" si="0"/>
         <v>0.57699999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -7280,26 +7301,26 @@
       <c r="C7" t="s">
         <v>243</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0.61</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>1</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0.01</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <f t="shared" si="0"/>
         <v>0.62</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
         <v>231</v>
       </c>
-      <c r="G13">
-        <f>SUM(G2:G12)</f>
+      <c r="H13">
+        <f>SUM(H2:H12)</f>
         <v>51.826999999999998</v>
       </c>
     </row>
@@ -7320,13 +7341,13 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>237</v>
       </c>
@@ -7340,7 +7361,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>181</v>
       </c>
@@ -7351,7 +7372,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>235</v>
       </c>
@@ -7359,18 +7380,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>239</v>
       </c>
       <c r="D5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>238</v>
       </c>
@@ -7383,7 +7404,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>231</v>
       </c>
@@ -7407,21 +7428,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -7432,7 +7453,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>142</v>
       </c>
@@ -7443,7 +7464,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>143</v>
       </c>
@@ -7454,27 +7475,27 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>154</v>
       </c>
@@ -7482,7 +7503,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>155</v>
       </c>
@@ -7493,7 +7514,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>157</v>
       </c>
@@ -7504,7 +7525,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>159</v>
       </c>
@@ -7512,7 +7533,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>172</v>
       </c>
@@ -7538,7 +7559,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
         <v>161</v>
       </c>
@@ -7564,7 +7585,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
         <v>165</v>
       </c>
@@ -7587,7 +7608,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>196</v>
       </c>
@@ -7613,7 +7634,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>167</v>
       </c>
@@ -7636,7 +7657,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>170</v>
       </c>
@@ -7659,7 +7680,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
         <v>186</v>
       </c>
@@ -7685,7 +7706,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
         <v>189</v>
       </c>
@@ -7711,7 +7732,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
         <v>192</v>
       </c>
@@ -7737,7 +7758,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
         <v>193</v>
       </c>
@@ -7763,7 +7784,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>198</v>
       </c>
@@ -7783,7 +7804,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>203</v>
       </c>
@@ -7806,7 +7827,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>208</v>
       </c>
@@ -7829,7 +7850,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>212</v>
       </c>
@@ -7852,7 +7873,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>215</v>
       </c>
@@ -7875,7 +7896,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>216</v>
       </c>
@@ -7898,7 +7919,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>220</v>
       </c>
@@ -7929,7 +7950,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding bulk of the components to the power schematic
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dktrfrd0/Documents/repos/binulator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francis\Documents\repos\binulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCC4787-C848-8748-93DB-881C9D283555}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FDA0B0-4EDE-4D81-84F1-F9701FCB95DB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12220" activeTab="3" xr2:uid="{DD5D3D6A-3E87-44D1-913F-F29D543648C7}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="12225" activeTab="4" xr2:uid="{DD5D3D6A-3E87-44D1-913F-F29D543648C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Keymap" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1367,27 +1368,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D03D7666-294F-443D-BB17-A232AE17218E}">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.5" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1"/>
-    <col min="10" max="10" width="16.5" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -1404,7 +1405,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>45</v>
       </c>
@@ -1442,7 +1443,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -1473,7 +1474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1504,7 +1505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1535,7 +1536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1566,7 +1567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1597,7 +1598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1628,7 +1629,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1659,7 +1660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1690,7 +1691,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1721,7 +1722,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1752,7 +1753,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1783,7 +1784,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1814,7 +1815,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1845,7 +1846,7 @@
         <v>C</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -1876,7 +1877,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1907,7 +1908,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1934,7 +1935,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1963,7 +1964,7 @@
         <v>=</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -2000,7 +2001,7 @@
         <v>+ (RL)</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -2037,7 +2038,7 @@
         <v>- (RR)</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -2074,7 +2075,7 @@
         <v>/ (&gt;&gt;)</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>* (&lt;&lt;)</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -2138,7 +2139,7 @@
         <v>%</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -2175,7 +2176,7 @@
         <v>| (~)</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -2212,7 +2213,7 @@
         <v>&amp; (^)</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -2239,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -2266,7 +2267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -2297,7 +2298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -2328,7 +2329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -2359,7 +2360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -2390,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>30</v>
       </c>
@@ -2421,7 +2422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>31</v>
       </c>
@@ -2452,7 +2453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>32</v>
       </c>
@@ -2483,7 +2484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>33</v>
       </c>
@@ -2524,7 +2525,7 @@
         <v>DEC (W8)</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>34</v>
       </c>
@@ -2565,7 +2566,7 @@
         <v>OCT (W16)</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>35</v>
       </c>
@@ -2606,7 +2607,7 @@
         <v>HEX (W32)</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>36</v>
       </c>
@@ -2647,7 +2648,7 @@
         <v>BIN (W64)</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>37</v>
       </c>
@@ -2680,7 +2681,7 @@
         <v>CS</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>38</v>
       </c>
@@ -2713,7 +2714,7 @@
         <v>CA</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>39</v>
       </c>
@@ -2754,7 +2755,7 @@
         <v>/\ (Menu)</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>40</v>
       </c>
@@ -2787,7 +2788,7 @@
         <v>\/</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>41</v>
       </c>
@@ -2820,7 +2821,7 @@
         <v>&lt;</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>42</v>
       </c>
@@ -2853,7 +2854,7 @@
         <v>&gt;</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43</v>
       </c>
@@ -2886,7 +2887,7 @@
         <v>R-&gt;A</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44</v>
       </c>
@@ -2919,7 +2920,7 @@
         <v>R-&gt;B</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>45</v>
       </c>
@@ -2952,7 +2953,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>46</v>
       </c>
@@ -2985,7 +2986,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>115</v>
       </c>
@@ -2994,7 +2995,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>116</v>
       </c>
@@ -3013,12 +3014,12 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="24" width="9.5" customWidth="1"/>
+    <col min="13" max="24" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -3026,7 +3027,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E5" s="6" t="s">
         <v>43</v>
       </c>
@@ -3100,7 +3101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
         <v>76</v>
       </c>
@@ -3165,7 +3166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
         <v>46</v>
       </c>
@@ -3227,7 +3228,7 @@
         <v>&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
         <v>6</v>
       </c>
@@ -3289,7 +3290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>3</v>
       </c>
@@ -3348,7 +3349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G10">
         <v>7</v>
       </c>
@@ -3413,7 +3414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G11">
         <v>4</v>
       </c>
@@ -3478,7 +3479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G12">
         <v>1</v>
       </c>
@@ -3543,7 +3544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G13">
         <v>0</v>
       </c>
@@ -3605,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M14" s="12">
         <f>VLOOKUP(A14,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -3655,7 +3656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M15" s="12">
         <f>VLOOKUP(A15,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -3705,7 +3706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M16" s="12">
         <f>VLOOKUP(A16,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -3755,7 +3756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M17" s="12">
         <f>VLOOKUP(A17,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -3805,7 +3806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M18" s="12">
         <f>VLOOKUP(A18,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -3855,7 +3856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M19" s="12">
         <f>VLOOKUP(A19,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -3905,7 +3906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M20" s="12">
         <f>VLOOKUP(A20,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -3955,7 +3956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M21" s="12">
         <f>VLOOKUP(A21,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4005,7 +4006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M22" s="12">
         <f>VLOOKUP(A22,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4055,7 +4056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M23" s="12">
         <f>VLOOKUP(A23,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4105,7 +4106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M24" s="12">
         <f>VLOOKUP(A24,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4155,7 +4156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M25" s="12">
         <f>VLOOKUP(A25,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4205,7 +4206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M26" s="12">
         <f>VLOOKUP(A26,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4255,7 +4256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M27" s="12">
         <f>VLOOKUP(A27,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4305,7 +4306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M28" s="12">
         <f>VLOOKUP(A28,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4355,7 +4356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M29" s="12">
         <f>VLOOKUP(A29,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4405,7 +4406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M30" s="12">
         <f>VLOOKUP(A30,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4455,7 +4456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M31" s="12">
         <f>VLOOKUP(A31,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4505,7 +4506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M32" s="12">
         <f>VLOOKUP(A32,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4555,7 +4556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="33" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M33" s="12">
         <f>VLOOKUP(A33,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4605,7 +4606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="34" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M34" s="12">
         <f>VLOOKUP(A34,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4655,7 +4656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="35" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M35">
         <f>VLOOKUP(A35,Keymap!$D$3:$L$49,9,0)</f>
         <v>0</v>
@@ -4705,7 +4706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="36" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M36">
         <f>VLOOKUP(A36,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -4751,7 +4752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="37" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M37">
         <f>VLOOKUP(A37,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -4797,7 +4798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="38" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M38">
         <f>VLOOKUP(A38,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -4843,7 +4844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="39" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M39">
         <f>VLOOKUP(A39,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -4889,7 +4890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="40" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M40">
         <f>VLOOKUP(A40,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -4935,7 +4936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="41" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M41">
         <f>VLOOKUP(A41,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -4981,7 +4982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="42" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M42">
         <f>VLOOKUP(A42,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5027,7 +5028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="43" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M43">
         <f>VLOOKUP(A43,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5073,7 +5074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="44" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M44">
         <f>VLOOKUP(A44,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5119,7 +5120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="45" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M45">
         <f>VLOOKUP(A45,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5165,7 +5166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="46" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M46">
         <f>VLOOKUP(A46,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5211,7 +5212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="47" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M47">
         <f>VLOOKUP(A47,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5257,7 +5258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="13:24" x14ac:dyDescent="0.2">
+    <row r="48" spans="13:24" x14ac:dyDescent="0.25">
       <c r="M48">
         <f>VLOOKUP(A48,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5303,7 +5304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="49" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M49">
         <f>VLOOKUP(A49,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5349,7 +5350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="50" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M50">
         <f>VLOOKUP(A50,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5395,7 +5396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="51" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M51">
         <f>VLOOKUP(A51,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5441,7 +5442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="52" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M52">
         <f>VLOOKUP(A52,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5487,7 +5488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="53" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M53">
         <f>VLOOKUP(A53,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5533,7 +5534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="54" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M54">
         <f>VLOOKUP(A54,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5579,7 +5580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="55" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M55">
         <f>VLOOKUP(A55,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5625,7 +5626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="56" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M56">
         <f>VLOOKUP(A56,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5671,7 +5672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="57" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M57">
         <f>VLOOKUP(A57,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5717,7 +5718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="58" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M58">
         <f>VLOOKUP(A58,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5763,7 +5764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="59" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M59">
         <f>VLOOKUP(A59,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5809,7 +5810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="60" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M60">
         <f>VLOOKUP(A60,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5855,7 +5856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="61" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M61">
         <f>VLOOKUP(A61,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5901,7 +5902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="62" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M62">
         <f>VLOOKUP(A62,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5947,7 +5948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="63" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M63">
         <f>VLOOKUP(A63,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -5993,7 +5994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="64" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M64">
         <f>VLOOKUP(A64,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6039,7 +6040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="65" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M65">
         <f>VLOOKUP(A65,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6085,7 +6086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="66" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M66">
         <f>VLOOKUP(A66,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6131,7 +6132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="67" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M67">
         <f>VLOOKUP(A67,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6177,7 +6178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="68" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M68">
         <f>VLOOKUP(A68,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6223,7 +6224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="69" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M69">
         <f>VLOOKUP(A69,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6269,7 +6270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="70" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M70">
         <f>VLOOKUP(A70,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6315,7 +6316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="71" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M71">
         <f>VLOOKUP(A71,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6361,7 +6362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="72" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M72">
         <f>VLOOKUP(A72,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6407,7 +6408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="73" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M73">
         <f>VLOOKUP(A73,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6453,7 +6454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="74" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M74">
         <f>VLOOKUP(A74,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6499,7 +6500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="75" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M75">
         <f>VLOOKUP(A75,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6545,7 +6546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="76" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M76">
         <f>VLOOKUP(A76,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6591,7 +6592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="77" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M77">
         <f>VLOOKUP(A77,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6637,7 +6638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="78" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M78">
         <f>VLOOKUP(A78,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6683,7 +6684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="79" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M79">
         <f>VLOOKUP(A79,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6729,7 +6730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="80" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M80">
         <f>VLOOKUP(A80,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6775,7 +6776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="81" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M81">
         <f>VLOOKUP(A81,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6821,7 +6822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="82" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M82">
         <f>VLOOKUP(A82,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6867,7 +6868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="83" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M83">
         <f>VLOOKUP(A83,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6913,7 +6914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="84" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M84">
         <f>VLOOKUP(A84,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -6959,7 +6960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="85" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M85">
         <f>VLOOKUP(A85,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -7005,7 +7006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="13:23" x14ac:dyDescent="0.2">
+    <row r="86" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M86">
         <f>VLOOKUP(A86,Keymap!$D$3:$L$49,8,0)</f>
         <v>0</v>
@@ -7060,14 +7061,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11910E8F-F881-4FEF-8DE8-B91E27082970}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -7081,7 +7084,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>117</v>
       </c>
@@ -7093,7 +7096,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>122</v>
       </c>
@@ -7104,7 +7107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>123</v>
       </c>
@@ -7122,23 +7125,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EF524C-A33F-43D3-860D-46F0F9167D43}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="67.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="182.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="182.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="182.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="182.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>132</v>
       </c>
@@ -7164,14 +7167,14 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>150</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="17" t="s">
         <v>149</v>
       </c>
       <c r="E2">
@@ -7188,7 +7191,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -7215,7 +7218,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -7240,7 +7243,7 @@
         <v>7.56</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -7267,7 +7270,7 @@
         <v>9.07</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -7291,7 +7294,7 @@
         <v>0.57699999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -7315,7 +7318,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
         <v>231</v>
       </c>
@@ -7327,9 +7330,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{62094591-22EE-4986-A182-297BA690668C}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{FA68F427-2C21-4093-B806-B39C39DB5E53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -7337,17 +7341,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113F1A7A-9196-48A1-BEB8-1076D278492A}">
   <dimension ref="A2:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>237</v>
       </c>
@@ -7361,7 +7365,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>181</v>
       </c>
@@ -7372,7 +7376,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>235</v>
       </c>
@@ -7380,18 +7384,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>239</v>
       </c>
       <c r="D5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>238</v>
       </c>
@@ -7404,7 +7408,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>231</v>
       </c>
@@ -7426,23 +7430,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86508168-602A-4B3E-8914-51A2FB7F6D83}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:D20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -7453,7 +7459,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>142</v>
       </c>
@@ -7464,7 +7470,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>143</v>
       </c>
@@ -7475,27 +7481,27 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>154</v>
       </c>
@@ -7503,7 +7509,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>155</v>
       </c>
@@ -7514,7 +7520,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>157</v>
       </c>
@@ -7525,7 +7531,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>159</v>
       </c>
@@ -7533,7 +7539,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>172</v>
       </c>
@@ -7559,7 +7565,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>161</v>
       </c>
@@ -7585,7 +7591,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>165</v>
       </c>
@@ -7608,7 +7614,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>196</v>
       </c>
@@ -7634,7 +7640,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>167</v>
       </c>
@@ -7657,7 +7663,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>170</v>
       </c>
@@ -7680,7 +7686,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>186</v>
       </c>
@@ -7706,7 +7712,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>189</v>
       </c>
@@ -7732,7 +7738,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>192</v>
       </c>
@@ -7758,7 +7764,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>193</v>
       </c>
@@ -7784,7 +7790,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>198</v>
       </c>
@@ -7804,7 +7810,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>203</v>
       </c>
@@ -7827,7 +7833,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>208</v>
       </c>
@@ -7850,7 +7856,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>212</v>
       </c>
@@ -7873,7 +7879,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>215</v>
       </c>
@@ -7896,7 +7902,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>216</v>
       </c>
@@ -7919,7 +7925,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>220</v>
       </c>
@@ -7950,7 +7956,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add calculations for the BQ24230 battery charger
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francis\Documents\repos\binulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FDA0B0-4EDE-4D81-84F1-F9701FCB95DB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FDFF02-7BF3-4694-A5B6-3A748C8A3130}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="12225" activeTab="4" xr2:uid="{DD5D3D6A-3E87-44D1-913F-F29D543648C7}"/>
+    <workbookView xWindow="30435" yWindow="3420" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{DD5D3D6A-3E87-44D1-913F-F29D543648C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Keymap" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="Pin Count" sheetId="4" r:id="rId3"/>
     <sheet name="BOM" sheetId="2" r:id="rId4"/>
     <sheet name="power estimate" sheetId="7" r:id="rId5"/>
-    <sheet name="display layout" sheetId="6" r:id="rId6"/>
-    <sheet name="Pin Mux" sheetId="3" r:id="rId7"/>
+    <sheet name="battery" sheetId="8" r:id="rId6"/>
+    <sheet name="display layout" sheetId="6" r:id="rId7"/>
+    <sheet name="Pin Mux" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="262">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -813,6 +814,51 @@
   </si>
   <si>
     <t>https://cdn-shop.adafruit.com/datasheets/62684.pdf</t>
+  </si>
+  <si>
+    <t>https://www.jaycar.com.au/18650-2600mah-li-ion-protected-battery/p/SB2299</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>mAh</t>
+  </si>
+  <si>
+    <t>advised charge rate</t>
+  </si>
+  <si>
+    <t>cut-off charging</t>
+  </si>
+  <si>
+    <t>cut-off discharging</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>max charge current</t>
+  </si>
+  <si>
+    <t>mA</t>
+  </si>
+  <si>
+    <t>target charge current</t>
+  </si>
+  <si>
+    <t>Kiset</t>
+  </si>
+  <si>
+    <t>Riset</t>
+  </si>
+  <si>
+    <t>ohms</t>
+  </si>
+  <si>
+    <t>Riset(nominal)</t>
+  </si>
+  <si>
+    <t>kohms</t>
   </si>
 </sst>
 </file>
@@ -7341,7 +7387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113F1A7A-9196-48A1-BEB8-1076D278492A}">
   <dimension ref="A2:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
@@ -7427,6 +7473,139 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94CFC39-4607-4B16-8FCF-9254461C13AB}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B3">
+        <v>2600</v>
+      </c>
+      <c r="C3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B4">
+        <v>0.2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B5">
+        <v>4.2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B6">
+        <v>2.75</v>
+      </c>
+      <c r="C6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B7">
+        <f>B3*B4</f>
+        <v>520</v>
+      </c>
+      <c r="C7" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B8">
+        <v>500</v>
+      </c>
+      <c r="C8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>256</v>
+      </c>
+      <c r="B9">
+        <f>B8/1000</f>
+        <v>0.5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>257</v>
+      </c>
+      <c r="B10">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>258</v>
+      </c>
+      <c r="B11">
+        <f>B10/B9</f>
+        <v>1740</v>
+      </c>
+      <c r="C11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>260</v>
+      </c>
+      <c r="B12">
+        <v>1.8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86508168-602A-4B3E-8914-51A2FB7F6D83}">
   <dimension ref="A1:H40"/>
   <sheetViews>
@@ -7950,7 +8129,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895AF181-FBD3-4423-B9E0-C4D4707FE481}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>